<commit_message>
py and data update
</commit_message>
<xml_diff>
--- a/data/Resolvable_Lakes.xlsx
+++ b/data/Resolvable_Lakes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\deqhq1\WQ-Share\Harmful Algal Blooms Coordination Team\HAB_Shiny_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D858283-B1C1-4014-9B55-9FA5EC5911D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D02023-F295-4478-8434-738146F28F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cyan_resolvable_lakes" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="177">
   <si>
     <t>GNIS_ID</t>
   </si>
@@ -559,6 +559,15 @@
   </si>
   <si>
     <t>Brownlee Reservoir_00378278</t>
+  </si>
+  <si>
+    <t>Ross Island Lagoon</t>
+  </si>
+  <si>
+    <t>Willamette River (Marquam Brg to St. Johns Brg)</t>
+  </si>
+  <si>
+    <t>NonResolvable</t>
   </si>
 </sst>
 </file>
@@ -885,11 +894,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -903,9 +912,10 @@
     <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -933,8 +943,11 @@
       <c r="I1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -948,7 +961,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -977,7 +990,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -1006,7 +1019,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>171</v>
       </c>
@@ -1027,7 +1040,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1056,7 +1069,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1085,7 +1098,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1114,7 +1127,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1143,7 +1156,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1172,7 +1185,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -1201,7 +1214,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -1230,7 +1243,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1259,7 +1272,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1288,7 +1301,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -1317,7 +1330,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2229,7 +2242,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>73</v>
       </c>
@@ -2258,7 +2271,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -2287,7 +2300,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>20</v>
       </c>
@@ -2316,7 +2329,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -2345,7 +2358,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>75</v>
       </c>
@@ -2374,7 +2387,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>76</v>
       </c>
@@ -2401,6 +2414,34 @@
       </c>
       <c r="I54" t="s">
         <v>154</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>174</v>
+      </c>
+      <c r="C55" t="s">
+        <v>174</v>
+      </c>
+      <c r="D55" t="s">
+        <v>155</v>
+      </c>
+      <c r="J55" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>175</v>
+      </c>
+      <c r="C56" t="s">
+        <v>175</v>
+      </c>
+      <c r="D56" t="s">
+        <v>155</v>
+      </c>
+      <c r="J56" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data updated till 7/10/2022
</commit_message>
<xml_diff>
--- a/data/Resolvable_Lakes.xlsx
+++ b/data/Resolvable_Lakes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\deqhq1\WQ-Share\Harmful Algal Blooms Coordination Team\HAB_Shiny_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D02023-F295-4478-8434-738146F28F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E6EEF9-3CB8-4D99-A5E5-6E5766086B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-13068" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cyan_resolvable_lakes" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="184">
   <si>
     <t>GNIS_ID</t>
   </si>
@@ -564,10 +564,31 @@
     <t>Ross Island Lagoon</t>
   </si>
   <si>
-    <t>Willamette River (Marquam Brg to St. Johns Brg)</t>
-  </si>
-  <si>
     <t>NonResolvable</t>
+  </si>
+  <si>
+    <t>Willamette River (Sellwood Brg to Willamette Falls)</t>
+  </si>
+  <si>
+    <t>Lemolo Lake_01144938</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Requested by Hannah LaGassey (USFS) on 6/23/2022.</t>
+  </si>
+  <si>
+    <t>01144938</t>
+  </si>
+  <si>
+    <t>Willamette River (Marquam Brg to Multnomah Channel)</t>
+  </si>
+  <si>
+    <t>*Lemolo Lake</t>
+  </si>
+  <si>
+    <t>*Lemolo Lake_01144938</t>
   </si>
 </sst>
 </file>
@@ -894,11 +915,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
+      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,10 +933,10 @@
     <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -944,10 +965,13 @@
         <v>170</v>
       </c>
       <c r="J1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="K1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -961,7 +985,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -990,7 +1014,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -1019,7 +1043,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>171</v>
       </c>
@@ -1040,7 +1064,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1069,7 +1093,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1098,7 +1122,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1127,7 +1151,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1156,7 +1180,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1185,7 +1209,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -1214,7 +1238,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -1243,7 +1267,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1272,7 +1296,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1301,7 +1325,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -1330,7 +1354,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2242,7 +2266,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>73</v>
       </c>
@@ -2271,7 +2295,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -2300,7 +2324,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>20</v>
       </c>
@@ -2329,7 +2353,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -2358,7 +2382,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>75</v>
       </c>
@@ -2387,7 +2411,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>76</v>
       </c>
@@ -2416,7 +2440,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>174</v>
       </c>
@@ -2430,18 +2454,55 @@
         <v>174</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C56" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D56" t="s">
         <v>155</v>
       </c>
       <c r="J56" t="s">
-        <v>175</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>176</v>
+      </c>
+      <c r="C57" t="s">
+        <v>176</v>
+      </c>
+      <c r="D57" t="s">
+        <v>155</v>
+      </c>
+      <c r="J57" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>182</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C58" t="s">
+        <v>177</v>
+      </c>
+      <c r="D58" t="s">
+        <v>155</v>
+      </c>
+      <c r="I58" t="s">
+        <v>183</v>
+      </c>
+      <c r="J58" t="s">
+        <v>177</v>
+      </c>
+      <c r="K58" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initials for V5 Data
</commit_message>
<xml_diff>
--- a/data/Resolvable_Lakes.xlsx
+++ b/data/Resolvable_Lakes.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\deqhq1\WQ-Share\Harmful Algal Blooms Coordination Team\HAB_Shiny_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1D5269-B2FD-406C-B0B5-D2912735F693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC59949-02E5-42DF-B29B-91A078EB06A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-13068" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23016" yWindow="-13008" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cyan_resolvable_lakes" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cyan_resolvable_lakes!$A$1:$N$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cyan_resolvable_lakes!$A$1:$O$65</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="227">
   <si>
     <t>GNIS_ID</t>
   </si>
@@ -715,13 +715,16 @@
   </si>
   <si>
     <t>Lake Billy Chinook (Crooked)_01138120</t>
+  </si>
+  <si>
+    <t>Area_Total_Cells</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -739,6 +742,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -770,13 +779,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,74 +1065,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N65"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="7" width="28.33203125" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="8" width="28.33203125" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="43.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="45.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1134,20 +1145,23 @@
       <c r="C2" t="s">
         <v>156</v>
       </c>
-      <c r="D2" t="s">
-        <v>155</v>
+      <c r="D2">
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>196</v>
+        <v>155</v>
       </c>
       <c r="F2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" t="s">
         <v>184</v>
       </c>
-      <c r="G2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1157,35 +1171,38 @@
       <c r="C3" t="s">
         <v>121</v>
       </c>
-      <c r="D3" t="s">
-        <v>155</v>
+      <c r="D3">
+        <v>164</v>
       </c>
       <c r="E3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" t="s">
         <v>197</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>184</v>
       </c>
-      <c r="G3" t="s">
-        <v>198</v>
-      </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I3">
         <v>8.32</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>87.9</v>
       </c>
-      <c r="J3" t="s">
-        <v>166</v>
-      </c>
       <c r="K3" t="s">
+        <v>166</v>
+      </c>
+      <c r="L3" t="s">
         <v>163</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -1195,35 +1212,38 @@
       <c r="C4" t="s">
         <v>122</v>
       </c>
-      <c r="D4" t="s">
-        <v>155</v>
+      <c r="D4">
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>196</v>
+        <v>155</v>
       </c>
       <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
         <v>185</v>
       </c>
-      <c r="G4" t="s">
-        <v>198</v>
-      </c>
-      <c r="H4">
+      <c r="H4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4">
         <v>7.8</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>118.8</v>
       </c>
-      <c r="J4" t="s">
-        <v>166</v>
-      </c>
       <c r="K4" t="s">
+        <v>166</v>
+      </c>
+      <c r="L4" t="s">
         <v>163</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>201</v>
       </c>
@@ -1233,48 +1253,49 @@
       <c r="C5" t="s">
         <v>203</v>
       </c>
-      <c r="D5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D5">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" t="s">
         <v>188</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>203</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>173</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
+      <c r="D6">
+        <v>515</v>
+      </c>
+      <c r="E6" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6" t="s">
         <v>186</v>
       </c>
-      <c r="G6" t="s">
-        <v>198</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2" t="s">
+      <c r="H6" t="s">
+        <v>198</v>
+      </c>
+      <c r="M6" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1284,35 +1305,38 @@
       <c r="C7" t="s">
         <v>54</v>
       </c>
-      <c r="D7" t="s">
-        <v>155</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="D7">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" t="s">
+        <v>196</v>
+      </c>
+      <c r="G7" t="s">
         <v>187</v>
       </c>
-      <c r="G7" t="s">
-        <v>198</v>
-      </c>
-      <c r="H7">
+      <c r="H7" t="s">
+        <v>198</v>
+      </c>
+      <c r="I7">
         <v>7.9</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>152</v>
       </c>
-      <c r="J7" t="s">
-        <v>166</v>
-      </c>
       <c r="K7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L7" t="s">
+        <v>168</v>
+      </c>
+      <c r="M7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1322,35 +1346,38 @@
       <c r="C8" t="s">
         <v>45</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
+        <v>196</v>
+      </c>
+      <c r="G8" t="s">
         <v>188</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>200</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>7.7</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>63</v>
       </c>
-      <c r="J8" t="s">
-        <v>166</v>
-      </c>
       <c r="K8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -1360,35 +1387,38 @@
       <c r="C9" t="s">
         <v>123</v>
       </c>
-      <c r="D9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="D9">
+        <v>180</v>
+      </c>
+      <c r="E9" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" t="s">
+        <v>196</v>
+      </c>
+      <c r="G9" t="s">
         <v>189</v>
       </c>
-      <c r="G9" t="s">
-        <v>198</v>
-      </c>
-      <c r="H9">
+      <c r="H9" t="s">
+        <v>198</v>
+      </c>
+      <c r="I9">
         <v>9.8000000000000007</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>42</v>
       </c>
-      <c r="J9" t="s">
-        <v>166</v>
-      </c>
       <c r="K9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L9" t="s">
+        <v>168</v>
+      </c>
+      <c r="M9" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1398,35 +1428,38 @@
       <c r="C10" t="s">
         <v>124</v>
       </c>
-      <c r="D10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="D10">
+        <v>578</v>
+      </c>
+      <c r="E10" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" t="s">
+        <v>196</v>
+      </c>
+      <c r="G10" t="s">
         <v>184</v>
       </c>
-      <c r="G10" t="s">
-        <v>198</v>
-      </c>
-      <c r="H10">
+      <c r="H10" t="s">
+        <v>198</v>
+      </c>
+      <c r="I10">
         <v>7.2</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>108</v>
       </c>
-      <c r="J10" t="s">
-        <v>166</v>
-      </c>
       <c r="K10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L10" t="s">
+        <v>168</v>
+      </c>
+      <c r="M10" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1436,35 +1469,38 @@
       <c r="C11" t="s">
         <v>125</v>
       </c>
-      <c r="D11" t="s">
-        <v>155</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>196</v>
+      <c r="D11">
+        <v>165</v>
+      </c>
+      <c r="E11" t="s">
+        <v>155</v>
       </c>
       <c r="F11" t="s">
+        <v>196</v>
+      </c>
+      <c r="G11" t="s">
         <v>189</v>
       </c>
-      <c r="G11" t="s">
-        <v>198</v>
-      </c>
-      <c r="H11">
+      <c r="H11" t="s">
+        <v>198</v>
+      </c>
+      <c r="I11">
         <v>7.6</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>26</v>
       </c>
-      <c r="J11" t="s">
-        <v>166</v>
-      </c>
       <c r="K11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L11" t="s">
+        <v>168</v>
+      </c>
+      <c r="M11" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -1474,35 +1510,38 @@
       <c r="C12" t="s">
         <v>126</v>
       </c>
-      <c r="D12" t="s">
-        <v>155</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>196</v>
+      <c r="D12">
+        <v>365</v>
+      </c>
+      <c r="E12" t="s">
+        <v>155</v>
       </c>
       <c r="F12" t="s">
+        <v>196</v>
+      </c>
+      <c r="G12" t="s">
         <v>190</v>
       </c>
-      <c r="G12" t="s">
-        <v>198</v>
-      </c>
-      <c r="H12">
+      <c r="H12" t="s">
+        <v>198</v>
+      </c>
+      <c r="I12">
         <v>8</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>142</v>
       </c>
-      <c r="J12" t="s">
-        <v>166</v>
-      </c>
       <c r="K12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L12" t="s">
+        <v>168</v>
+      </c>
+      <c r="M12" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>80</v>
       </c>
@@ -1512,35 +1551,38 @@
       <c r="C13" t="s">
         <v>127</v>
       </c>
-      <c r="D13" t="s">
-        <v>155</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>196</v>
+      <c r="D13">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>155</v>
       </c>
       <c r="F13" t="s">
+        <v>196</v>
+      </c>
+      <c r="G13" t="s">
         <v>189</v>
       </c>
-      <c r="G13" t="s">
-        <v>198</v>
-      </c>
-      <c r="H13">
+      <c r="H13" t="s">
+        <v>198</v>
+      </c>
+      <c r="I13">
         <v>7.5</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>18</v>
       </c>
-      <c r="J13" t="s">
-        <v>166</v>
-      </c>
       <c r="K13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L13" t="s">
+        <v>168</v>
+      </c>
+      <c r="M13" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1550,35 +1592,38 @@
       <c r="C14" t="s">
         <v>128</v>
       </c>
-      <c r="D14" t="s">
-        <v>155</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>196</v>
+      <c r="D14">
+        <v>135</v>
+      </c>
+      <c r="E14" t="s">
+        <v>155</v>
       </c>
       <c r="F14" t="s">
+        <v>196</v>
+      </c>
+      <c r="G14" t="s">
         <v>189</v>
       </c>
-      <c r="G14" t="s">
-        <v>198</v>
-      </c>
-      <c r="H14">
+      <c r="H14" t="s">
+        <v>198</v>
+      </c>
+      <c r="I14">
         <v>8.6999999999999993</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>38</v>
       </c>
-      <c r="J14" t="s">
-        <v>166</v>
-      </c>
       <c r="K14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L14" t="s">
+        <v>168</v>
+      </c>
+      <c r="M14" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1588,35 +1633,38 @@
       <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15">
+        <v>91</v>
+      </c>
+      <c r="E15" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F15" t="s">
+        <v>196</v>
+      </c>
+      <c r="G15" t="s">
         <v>188</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>200</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>0</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>34</v>
       </c>
-      <c r="J15" t="s">
-        <v>166</v>
-      </c>
       <c r="K15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L15" t="s">
+        <v>168</v>
+      </c>
+      <c r="M15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -1626,35 +1674,38 @@
       <c r="C16" t="s">
         <v>129</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
         <v>129</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F16" t="s">
+        <v>196</v>
+      </c>
+      <c r="G16" t="s">
         <v>188</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>200</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>7.6</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>47</v>
       </c>
-      <c r="J16" t="s">
-        <v>166</v>
-      </c>
       <c r="K16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L16" t="s">
+        <v>168</v>
+      </c>
+      <c r="M16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1664,35 +1715,38 @@
       <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17">
+        <v>137</v>
+      </c>
+      <c r="E17" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F17" t="s">
+        <v>196</v>
+      </c>
+      <c r="G17" t="s">
         <v>191</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>200</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>9.5</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>29</v>
       </c>
-      <c r="J17" t="s">
-        <v>166</v>
-      </c>
       <c r="K17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L17" t="s">
+        <v>168</v>
+      </c>
+      <c r="M17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1702,35 +1756,38 @@
       <c r="C18" t="s">
         <v>46</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18">
+        <v>49</v>
+      </c>
+      <c r="E18" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F18" t="s">
+        <v>196</v>
+      </c>
+      <c r="G18" t="s">
         <v>188</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>200</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>7.9</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>49</v>
       </c>
-      <c r="J18" t="s">
-        <v>166</v>
-      </c>
       <c r="K18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L18" t="s">
+        <v>168</v>
+      </c>
+      <c r="M18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -1740,35 +1797,38 @@
       <c r="C19" t="s">
         <v>130</v>
       </c>
-      <c r="D19" t="s">
-        <v>155</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>196</v>
+      <c r="D19">
+        <v>156</v>
+      </c>
+      <c r="E19" t="s">
+        <v>155</v>
       </c>
       <c r="F19" t="s">
+        <v>196</v>
+      </c>
+      <c r="G19" t="s">
         <v>192</v>
       </c>
-      <c r="G19" t="s">
-        <v>198</v>
-      </c>
-      <c r="H19">
+      <c r="H19" t="s">
+        <v>198</v>
+      </c>
+      <c r="I19">
         <v>7.5</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>85</v>
       </c>
-      <c r="J19" t="s">
-        <v>166</v>
-      </c>
       <c r="K19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L19" t="s">
+        <v>168</v>
+      </c>
+      <c r="M19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -1778,35 +1838,38 @@
       <c r="C20" t="s">
         <v>131</v>
       </c>
-      <c r="D20" t="s">
-        <v>155</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>196</v>
+      <c r="D20">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>155</v>
       </c>
       <c r="F20" t="s">
+        <v>196</v>
+      </c>
+      <c r="G20" t="s">
         <v>189</v>
       </c>
-      <c r="G20" t="s">
-        <v>198</v>
-      </c>
-      <c r="H20">
+      <c r="H20" t="s">
+        <v>198</v>
+      </c>
+      <c r="I20">
         <v>7.9</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>310</v>
       </c>
-      <c r="J20" t="s">
-        <v>166</v>
-      </c>
       <c r="K20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L20" t="s">
+        <v>168</v>
+      </c>
+      <c r="M20" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -1816,35 +1879,38 @@
       <c r="C21" t="s">
         <v>132</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
         <v>132</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F21" t="s">
+        <v>196</v>
+      </c>
+      <c r="G21" t="s">
         <v>188</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>200</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>7.8</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>37.299999999999997</v>
       </c>
-      <c r="J21" t="s">
-        <v>166</v>
-      </c>
       <c r="K21" t="s">
+        <v>166</v>
+      </c>
+      <c r="L21" t="s">
         <v>164</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1854,35 +1920,38 @@
       <c r="C22" t="s">
         <v>42</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22">
+        <v>294</v>
+      </c>
+      <c r="E22" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F22" t="s">
+        <v>196</v>
+      </c>
+      <c r="G22" t="s">
         <v>188</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>200</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>7.8</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>56.3</v>
       </c>
-      <c r="J22" t="s">
-        <v>166</v>
-      </c>
       <c r="K22" t="s">
+        <v>166</v>
+      </c>
+      <c r="L22" t="s">
         <v>164</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1892,35 +1961,38 @@
       <c r="C23" t="s">
         <v>49</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23">
+        <v>32</v>
+      </c>
+      <c r="E23" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F23" t="s">
+        <v>196</v>
+      </c>
+      <c r="G23" t="s">
         <v>188</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>200</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>7.2</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>42</v>
       </c>
-      <c r="J23" t="s">
-        <v>166</v>
-      </c>
       <c r="K23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L23" t="s">
+        <v>168</v>
+      </c>
+      <c r="M23" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -1930,35 +2002,38 @@
       <c r="C24" t="s">
         <v>133</v>
       </c>
-      <c r="D24" t="s">
-        <v>155</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>196</v>
+      <c r="D24">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
+        <v>155</v>
       </c>
       <c r="F24" t="s">
+        <v>196</v>
+      </c>
+      <c r="G24" t="s">
         <v>184</v>
       </c>
-      <c r="G24" t="s">
-        <v>198</v>
-      </c>
-      <c r="H24">
+      <c r="H24" t="s">
+        <v>198</v>
+      </c>
+      <c r="I24">
         <v>6.2</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>10.549999999999999</v>
       </c>
-      <c r="J24" t="s">
-        <v>166</v>
-      </c>
       <c r="K24" t="s">
+        <v>166</v>
+      </c>
+      <c r="L24" t="s">
         <v>165</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1968,35 +2043,38 @@
       <c r="C25" t="s">
         <v>134</v>
       </c>
-      <c r="D25" t="s">
-        <v>155</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>196</v>
+      <c r="D25">
+        <v>143</v>
+      </c>
+      <c r="E25" t="s">
+        <v>155</v>
       </c>
       <c r="F25" t="s">
+        <v>196</v>
+      </c>
+      <c r="G25" t="s">
         <v>184</v>
       </c>
-      <c r="G25" t="s">
-        <v>198</v>
-      </c>
-      <c r="H25">
+      <c r="H25" t="s">
+        <v>198</v>
+      </c>
+      <c r="I25">
         <v>7.3</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>54</v>
       </c>
-      <c r="J25" t="s">
-        <v>166</v>
-      </c>
       <c r="K25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L25" t="s">
+        <v>168</v>
+      </c>
+      <c r="M25" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -2006,32 +2084,35 @@
       <c r="C26" t="s">
         <v>135</v>
       </c>
-      <c r="D26" t="s">
-        <v>155</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>196</v>
+      <c r="D26">
+        <v>4178</v>
+      </c>
+      <c r="E26" t="s">
+        <v>155</v>
       </c>
       <c r="F26" t="s">
+        <v>196</v>
+      </c>
+      <c r="G26" t="s">
         <v>192</v>
       </c>
-      <c r="G26" t="s">
-        <v>198</v>
-      </c>
-      <c r="H26">
+      <c r="H26" t="s">
+        <v>198</v>
+      </c>
+      <c r="I26">
         <v>9.3000000000000007</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>2075</v>
       </c>
-      <c r="J26" t="s">
-        <v>166</v>
-      </c>
       <c r="K26" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+      <c r="L26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2041,35 +2122,38 @@
       <c r="C27" t="s">
         <v>52</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27">
+        <v>123</v>
+      </c>
+      <c r="E27" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F27" t="s">
+        <v>196</v>
+      </c>
+      <c r="G27" t="s">
         <v>188</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>200</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>7.3</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>34</v>
       </c>
-      <c r="J27" t="s">
-        <v>166</v>
-      </c>
       <c r="K27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L27" t="s">
+        <v>168</v>
+      </c>
+      <c r="M27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -2079,35 +2163,38 @@
       <c r="C28" t="s">
         <v>136</v>
       </c>
-      <c r="D28" t="s">
-        <v>155</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>196</v>
+      <c r="D28">
+        <v>317</v>
+      </c>
+      <c r="E28" t="s">
+        <v>155</v>
       </c>
       <c r="F28" t="s">
+        <v>196</v>
+      </c>
+      <c r="G28" t="s">
         <v>190</v>
       </c>
-      <c r="G28" t="s">
-        <v>198</v>
-      </c>
-      <c r="H28">
+      <c r="H28" t="s">
+        <v>198</v>
+      </c>
+      <c r="I28">
         <v>8</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>205</v>
       </c>
-      <c r="J28" t="s">
-        <v>166</v>
-      </c>
       <c r="K28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L28" t="s">
+        <v>168</v>
+      </c>
+      <c r="M28" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -2117,35 +2204,38 @@
       <c r="C29" t="s">
         <v>51</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29">
+        <v>40</v>
+      </c>
+      <c r="E29" t="s">
         <v>51</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F29" t="s">
+        <v>196</v>
+      </c>
+      <c r="G29" t="s">
         <v>188</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>199</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>6.6</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>64</v>
       </c>
-      <c r="J29" t="s">
-        <v>166</v>
-      </c>
       <c r="K29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L29" t="s">
+        <v>168</v>
+      </c>
+      <c r="M29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -2155,35 +2245,38 @@
       <c r="C30" t="s">
         <v>47</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30">
+        <v>81</v>
+      </c>
+      <c r="E30" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F30" t="s">
+        <v>196</v>
+      </c>
+      <c r="G30" t="s">
         <v>188</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>200</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>8.1</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>52</v>
       </c>
-      <c r="J30" t="s">
-        <v>166</v>
-      </c>
       <c r="K30" t="s">
+        <v>166</v>
+      </c>
+      <c r="L30" t="s">
         <v>165</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -2193,35 +2286,38 @@
       <c r="C31" t="s">
         <v>137</v>
       </c>
-      <c r="D31" t="s">
-        <v>155</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>196</v>
+      <c r="D31">
+        <v>69</v>
+      </c>
+      <c r="E31" t="s">
+        <v>155</v>
       </c>
       <c r="F31" t="s">
+        <v>196</v>
+      </c>
+      <c r="G31" t="s">
         <v>184</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>200</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>7.7</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>67</v>
       </c>
-      <c r="J31" t="s">
-        <v>166</v>
-      </c>
       <c r="K31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L31" t="s">
+        <v>168</v>
+      </c>
+      <c r="M31" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -2231,32 +2327,35 @@
       <c r="C32" t="s">
         <v>138</v>
       </c>
-      <c r="D32" t="s">
-        <v>155</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>196</v>
+      <c r="D32">
+        <v>1820</v>
+      </c>
+      <c r="E32" t="s">
+        <v>155</v>
       </c>
       <c r="F32" t="s">
+        <v>196</v>
+      </c>
+      <c r="G32" t="s">
         <v>190</v>
       </c>
-      <c r="G32" t="s">
-        <v>198</v>
-      </c>
-      <c r="H32">
+      <c r="H32" t="s">
+        <v>198</v>
+      </c>
+      <c r="I32">
         <v>10.1</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>42000</v>
       </c>
-      <c r="J32" t="s">
-        <v>166</v>
-      </c>
       <c r="K32" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+      <c r="L32" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -2266,35 +2365,38 @@
       <c r="C33" t="s">
         <v>139</v>
       </c>
-      <c r="D33" t="s">
-        <v>155</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>196</v>
+      <c r="D33">
+        <v>152</v>
+      </c>
+      <c r="E33" t="s">
+        <v>155</v>
       </c>
       <c r="F33" t="s">
+        <v>196</v>
+      </c>
+      <c r="G33" t="s">
         <v>189</v>
       </c>
-      <c r="G33" t="s">
-        <v>198</v>
-      </c>
-      <c r="H33">
+      <c r="H33" t="s">
+        <v>198</v>
+      </c>
+      <c r="I33">
         <v>9.4</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>164</v>
       </c>
-      <c r="J33" t="s">
-        <v>166</v>
-      </c>
       <c r="K33" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L33" t="s">
+        <v>168</v>
+      </c>
+      <c r="M33" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>217</v>
       </c>
@@ -2304,26 +2406,29 @@
       <c r="C34" t="s">
         <v>223</v>
       </c>
-      <c r="D34" t="s">
-        <v>155</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>196</v>
+      <c r="D34">
+        <v>77</v>
+      </c>
+      <c r="E34" t="s">
+        <v>155</v>
       </c>
       <c r="F34" t="s">
+        <v>196</v>
+      </c>
+      <c r="G34" t="s">
         <v>189</v>
       </c>
-      <c r="G34" t="s">
-        <v>198</v>
-      </c>
-      <c r="M34" t="s">
+      <c r="H34" t="s">
+        <v>198</v>
+      </c>
+      <c r="N34" t="s">
         <v>223</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>218</v>
       </c>
@@ -2333,26 +2438,29 @@
       <c r="C35" t="s">
         <v>224</v>
       </c>
-      <c r="D35" t="s">
-        <v>155</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>196</v>
+      <c r="D35">
+        <v>47</v>
+      </c>
+      <c r="E35" t="s">
+        <v>155</v>
       </c>
       <c r="F35" t="s">
+        <v>196</v>
+      </c>
+      <c r="G35" t="s">
         <v>189</v>
       </c>
-      <c r="G35" t="s">
-        <v>198</v>
-      </c>
-      <c r="M35" t="s">
+      <c r="H35" t="s">
+        <v>198</v>
+      </c>
+      <c r="N35" t="s">
         <v>224</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>219</v>
       </c>
@@ -2362,102 +2470,111 @@
       <c r="C36" t="s">
         <v>225</v>
       </c>
-      <c r="D36" t="s">
-        <v>155</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>196</v>
+      <c r="D36">
+        <v>28</v>
+      </c>
+      <c r="E36" t="s">
+        <v>155</v>
       </c>
       <c r="F36" t="s">
+        <v>196</v>
+      </c>
+      <c r="G36" t="s">
         <v>189</v>
       </c>
-      <c r="G36" t="s">
-        <v>198</v>
-      </c>
-      <c r="M36" t="s">
+      <c r="H36" t="s">
+        <v>198</v>
+      </c>
+      <c r="N36" t="s">
         <v>225</v>
       </c>
-      <c r="N36" t="s">
+      <c r="O36" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D37" t="s">
-        <v>155</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="D37" s="4">
+        <v>51</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="G37" t="s">
-        <v>198</v>
-      </c>
-      <c r="H37">
+      <c r="H37" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I37" s="4">
         <v>7.4</v>
       </c>
-      <c r="I37">
+      <c r="J37" s="4">
         <v>30</v>
       </c>
-      <c r="J37" t="s">
-        <v>166</v>
-      </c>
-      <c r="K37" t="s">
+      <c r="K37" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="L37" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="38" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D38" t="s">
-        <v>155</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="D38" s="4">
+        <v>431</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="G38" t="s">
-        <v>198</v>
-      </c>
-      <c r="H38">
+      <c r="H38" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I38" s="4">
         <v>8.4</v>
       </c>
-      <c r="I38">
+      <c r="J38" s="4">
         <v>217.5</v>
       </c>
-      <c r="J38" t="s">
-        <v>166</v>
-      </c>
-      <c r="K38" t="s">
+      <c r="K38" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="L38" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>158</v>
       </c>
@@ -2467,23 +2584,26 @@
       <c r="C39" t="s">
         <v>157</v>
       </c>
-      <c r="D39" t="s">
-        <v>155</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>196</v>
+      <c r="D39">
+        <v>656</v>
+      </c>
+      <c r="E39" t="s">
+        <v>155</v>
       </c>
       <c r="F39" t="s">
+        <v>196</v>
+      </c>
+      <c r="G39" t="s">
         <v>187</v>
       </c>
-      <c r="G39" t="s">
-        <v>198</v>
-      </c>
-      <c r="L39" t="s">
+      <c r="H39" t="s">
+        <v>198</v>
+      </c>
+      <c r="M39" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>206</v>
       </c>
@@ -2493,26 +2613,29 @@
       <c r="C40" t="s">
         <v>208</v>
       </c>
-      <c r="D40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>196</v>
+      <c r="D40">
+        <v>14</v>
+      </c>
+      <c r="E40" t="s">
+        <v>155</v>
       </c>
       <c r="F40" t="s">
+        <v>196</v>
+      </c>
+      <c r="G40" t="s">
         <v>189</v>
       </c>
-      <c r="G40" t="s">
-        <v>198</v>
-      </c>
-      <c r="M40" t="s">
+      <c r="H40" t="s">
+        <v>198</v>
+      </c>
+      <c r="N40" t="s">
         <v>208</v>
       </c>
-      <c r="N40" t="s">
+      <c r="O40" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>205</v>
       </c>
@@ -2522,26 +2645,29 @@
       <c r="C41" t="s">
         <v>177</v>
       </c>
-      <c r="D41" t="s">
-        <v>155</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>196</v>
+      <c r="D41">
+        <v>17</v>
+      </c>
+      <c r="E41" t="s">
+        <v>155</v>
       </c>
       <c r="F41" t="s">
+        <v>196</v>
+      </c>
+      <c r="G41" t="s">
         <v>191</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>200</v>
       </c>
-      <c r="M41" t="s">
+      <c r="N41" t="s">
         <v>177</v>
       </c>
-      <c r="N41" t="s">
+      <c r="O41" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -2551,35 +2677,38 @@
       <c r="C42" t="s">
         <v>48</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42">
+        <v>122</v>
+      </c>
+      <c r="E42" t="s">
         <v>48</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F42" t="s">
+        <v>196</v>
+      </c>
+      <c r="G42" t="s">
         <v>191</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>200</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>7.7</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>48</v>
       </c>
-      <c r="J42" t="s">
-        <v>166</v>
-      </c>
       <c r="K42" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L42" t="s">
+        <v>168</v>
+      </c>
+      <c r="M42" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -2589,35 +2718,38 @@
       <c r="C43" t="s">
         <v>142</v>
       </c>
-      <c r="D43" t="s">
-        <v>155</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>196</v>
+      <c r="D43">
+        <v>1284</v>
+      </c>
+      <c r="E43" t="s">
+        <v>155</v>
       </c>
       <c r="F43" t="s">
+        <v>196</v>
+      </c>
+      <c r="G43" t="s">
         <v>190</v>
       </c>
-      <c r="G43" t="s">
-        <v>198</v>
-      </c>
-      <c r="H43">
+      <c r="H43" t="s">
+        <v>198</v>
+      </c>
+      <c r="I43">
         <v>7.8</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>503</v>
       </c>
-      <c r="J43" t="s">
-        <v>166</v>
-      </c>
       <c r="K43" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L43" t="s">
+        <v>168</v>
+      </c>
+      <c r="M43" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -2627,35 +2759,38 @@
       <c r="C44" t="s">
         <v>143</v>
       </c>
-      <c r="D44" t="s">
-        <v>155</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>196</v>
+      <c r="D44">
+        <v>27</v>
+      </c>
+      <c r="E44" t="s">
+        <v>155</v>
       </c>
       <c r="F44" t="s">
+        <v>196</v>
+      </c>
+      <c r="G44" t="s">
         <v>187</v>
       </c>
-      <c r="G44" t="s">
-        <v>198</v>
-      </c>
-      <c r="H44">
+      <c r="H44" t="s">
+        <v>198</v>
+      </c>
+      <c r="I44">
         <v>8.8000000000000007</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>76</v>
       </c>
-      <c r="J44" t="s">
-        <v>166</v>
-      </c>
       <c r="K44" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L44" t="s">
+        <v>168</v>
+      </c>
+      <c r="M44" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>214</v>
       </c>
@@ -2665,31 +2800,29 @@
       <c r="C45" t="s">
         <v>216</v>
       </c>
-      <c r="D45" t="s">
-        <v>155</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>196</v>
+      <c r="D45">
+        <v>34</v>
+      </c>
+      <c r="E45" t="s">
+        <v>155</v>
       </c>
       <c r="F45" t="s">
+        <v>196</v>
+      </c>
+      <c r="G45" t="s">
         <v>189</v>
       </c>
-      <c r="G45" t="s">
-        <v>198</v>
-      </c>
-      <c r="H45"/>
-      <c r="I45"/>
-      <c r="J45"/>
-      <c r="K45"/>
-      <c r="L45"/>
-      <c r="M45" t="s">
+      <c r="H45" t="s">
+        <v>198</v>
+      </c>
+      <c r="N45" t="s">
         <v>216</v>
       </c>
-      <c r="N45" t="s">
+      <c r="O45" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>68</v>
       </c>
@@ -2699,35 +2832,38 @@
       <c r="C46" t="s">
         <v>144</v>
       </c>
-      <c r="D46" t="s">
-        <v>155</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>196</v>
+      <c r="D46">
+        <v>152</v>
+      </c>
+      <c r="E46" t="s">
+        <v>155</v>
       </c>
       <c r="F46" t="s">
+        <v>196</v>
+      </c>
+      <c r="G46" t="s">
         <v>189</v>
       </c>
-      <c r="G46" t="s">
-        <v>198</v>
-      </c>
-      <c r="H46">
+      <c r="H46" t="s">
+        <v>198</v>
+      </c>
+      <c r="I46">
         <v>9.3000000000000007</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>35.200000000000003</v>
       </c>
-      <c r="J46" t="s">
-        <v>166</v>
-      </c>
       <c r="K46" t="s">
+        <v>166</v>
+      </c>
+      <c r="L46" t="s">
         <v>164</v>
       </c>
-      <c r="L46" t="s">
+      <c r="M46" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>69</v>
       </c>
@@ -2737,35 +2873,38 @@
       <c r="C47" t="s">
         <v>145</v>
       </c>
-      <c r="D47" t="s">
-        <v>155</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>196</v>
+      <c r="D47">
+        <v>58</v>
+      </c>
+      <c r="E47" t="s">
+        <v>155</v>
       </c>
       <c r="F47" t="s">
+        <v>196</v>
+      </c>
+      <c r="G47" t="s">
         <v>189</v>
       </c>
-      <c r="G47" t="s">
-        <v>198</v>
-      </c>
-      <c r="H47">
+      <c r="H47" t="s">
+        <v>198</v>
+      </c>
+      <c r="I47">
         <v>8.5</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>560</v>
       </c>
-      <c r="J47" t="s">
-        <v>166</v>
-      </c>
       <c r="K47" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L47" t="s">
+        <v>168</v>
+      </c>
+      <c r="M47" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>210</v>
       </c>
@@ -2775,26 +2914,29 @@
       <c r="C48" t="s">
         <v>212</v>
       </c>
-      <c r="D48" t="s">
-        <v>155</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>196</v>
+      <c r="D48">
+        <v>93</v>
+      </c>
+      <c r="E48" t="s">
+        <v>155</v>
       </c>
       <c r="F48" t="s">
+        <v>196</v>
+      </c>
+      <c r="G48" t="s">
         <v>189</v>
       </c>
-      <c r="G48" t="s">
-        <v>198</v>
-      </c>
-      <c r="M48" t="s">
+      <c r="H48" t="s">
+        <v>198</v>
+      </c>
+      <c r="N48" t="s">
         <v>212</v>
       </c>
-      <c r="N48" t="s">
+      <c r="O48" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -2804,48 +2946,52 @@
       <c r="C49" t="s">
         <v>146</v>
       </c>
-      <c r="D49" t="s">
-        <v>155</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>196</v>
+      <c r="D49">
+        <v>21</v>
+      </c>
+      <c r="E49" t="s">
+        <v>155</v>
       </c>
       <c r="F49" t="s">
+        <v>196</v>
+      </c>
+      <c r="G49" t="s">
         <v>192</v>
       </c>
-      <c r="G49" t="s">
-        <v>198</v>
-      </c>
-      <c r="L49" t="s">
+      <c r="H49" t="s">
+        <v>198</v>
+      </c>
+      <c r="M49" t="s">
         <v>146</v>
       </c>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-    </row>
-    <row r="50" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>174</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" t="s">
         <v>174</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F50" s="2" t="s">
+      <c r="D50">
+        <v>31</v>
+      </c>
+      <c r="E50" t="s">
+        <v>155</v>
+      </c>
+      <c r="F50" t="s">
+        <v>196</v>
+      </c>
+      <c r="G50" t="s">
         <v>188</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="H50" t="s">
         <v>199</v>
       </c>
-      <c r="M50" s="2" t="s">
+      <c r="N50" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>27</v>
       </c>
@@ -2855,35 +3001,38 @@
       <c r="C51" t="s">
         <v>41</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51">
+        <v>120</v>
+      </c>
+      <c r="E51" t="s">
         <v>41</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F51" t="s">
+        <v>196</v>
+      </c>
+      <c r="G51" t="s">
         <v>193</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>200</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>8.3000000000000007</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <v>72</v>
       </c>
-      <c r="J51" t="s">
-        <v>166</v>
-      </c>
       <c r="K51" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L51" t="s">
+        <v>168</v>
+      </c>
+      <c r="M51" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -2893,35 +3042,38 @@
       <c r="C52" t="s">
         <v>40</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52">
+        <v>126</v>
+      </c>
+      <c r="E52" t="s">
         <v>40</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F52" t="s">
+        <v>196</v>
+      </c>
+      <c r="G52" t="s">
         <v>188</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>199</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>0</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>106</v>
       </c>
-      <c r="J52" t="s">
-        <v>166</v>
-      </c>
       <c r="K52" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L52" t="s">
+        <v>168</v>
+      </c>
+      <c r="M52" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>71</v>
       </c>
@@ -2931,32 +3083,35 @@
       <c r="C53" t="s">
         <v>147</v>
       </c>
-      <c r="D53" t="s">
-        <v>155</v>
+      <c r="D53">
+        <v>1211</v>
       </c>
       <c r="E53" t="s">
+        <v>155</v>
+      </c>
+      <c r="F53" t="s">
         <v>197</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>190</v>
       </c>
-      <c r="G53" t="s">
-        <v>198</v>
-      </c>
-      <c r="H53">
+      <c r="H53" t="s">
+        <v>198</v>
+      </c>
+      <c r="I53">
         <v>9.6999999999999993</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>7000</v>
       </c>
-      <c r="J53" t="s">
-        <v>166</v>
-      </c>
       <c r="K53" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+      <c r="L53" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -2966,35 +3121,38 @@
       <c r="C54" t="s">
         <v>148</v>
       </c>
-      <c r="D54" t="s">
-        <v>155</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>196</v>
+      <c r="D54">
+        <v>29</v>
+      </c>
+      <c r="E54" t="s">
+        <v>155</v>
       </c>
       <c r="F54" t="s">
+        <v>196</v>
+      </c>
+      <c r="G54" t="s">
         <v>189</v>
       </c>
-      <c r="G54" t="s">
-        <v>198</v>
-      </c>
-      <c r="H54">
+      <c r="H54" t="s">
+        <v>198</v>
+      </c>
+      <c r="I54">
         <v>6.7</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>6</v>
       </c>
-      <c r="J54" t="s">
-        <v>166</v>
-      </c>
       <c r="K54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L54" t="s">
+        <v>168</v>
+      </c>
+      <c r="M54" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -3004,23 +3162,26 @@
       <c r="C55" t="s">
         <v>149</v>
       </c>
-      <c r="D55" t="s">
-        <v>155</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>196</v>
+      <c r="D55">
+        <v>38</v>
+      </c>
+      <c r="E55" t="s">
+        <v>155</v>
       </c>
       <c r="F55" t="s">
+        <v>196</v>
+      </c>
+      <c r="G55" t="s">
         <v>190</v>
       </c>
-      <c r="G55" t="s">
-        <v>198</v>
-      </c>
-      <c r="L55" t="s">
+      <c r="H55" t="s">
+        <v>198</v>
+      </c>
+      <c r="M55" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>83</v>
       </c>
@@ -3030,35 +3191,38 @@
       <c r="C56" t="s">
         <v>150</v>
       </c>
-      <c r="D56" t="s">
-        <v>155</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>196</v>
+      <c r="D56">
+        <v>27</v>
+      </c>
+      <c r="E56" t="s">
+        <v>155</v>
       </c>
       <c r="F56" t="s">
+        <v>196</v>
+      </c>
+      <c r="G56" t="s">
         <v>186</v>
       </c>
-      <c r="G56" t="s">
-        <v>198</v>
-      </c>
-      <c r="H56">
+      <c r="H56" t="s">
+        <v>198</v>
+      </c>
+      <c r="I56">
         <v>8.4</v>
       </c>
-      <c r="I56">
+      <c r="J56">
         <v>210</v>
       </c>
-      <c r="J56" t="s">
-        <v>166</v>
-      </c>
       <c r="K56" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L56" t="s">
+        <v>168</v>
+      </c>
+      <c r="M56" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -3068,35 +3232,38 @@
       <c r="C57" t="s">
         <v>53</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57">
         <v>53</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>196</v>
+      <c r="E57" t="s">
+        <v>53</v>
       </c>
       <c r="F57" t="s">
+        <v>196</v>
+      </c>
+      <c r="G57" t="s">
         <v>188</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>199</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <v>7.3</v>
       </c>
-      <c r="I57">
+      <c r="J57">
         <v>49</v>
       </c>
-      <c r="J57" t="s">
-        <v>166</v>
-      </c>
       <c r="K57" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L57" t="s">
+        <v>168</v>
+      </c>
+      <c r="M57" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -3106,32 +3273,35 @@
       <c r="C58" t="s">
         <v>167</v>
       </c>
-      <c r="D58" t="s">
-        <v>155</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="D58">
+        <v>42</v>
+      </c>
+      <c r="E58" t="s">
+        <v>155</v>
+      </c>
+      <c r="G58" t="s">
         <v>185</v>
       </c>
-      <c r="G58" t="s">
-        <v>198</v>
-      </c>
-      <c r="H58">
+      <c r="H58" t="s">
+        <v>198</v>
+      </c>
+      <c r="I58">
         <v>7.8</v>
       </c>
-      <c r="I58">
+      <c r="J58">
         <v>148</v>
       </c>
-      <c r="J58" t="s">
-        <v>166</v>
-      </c>
       <c r="K58" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L58" t="s">
+        <v>168</v>
+      </c>
+      <c r="M58" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -3141,35 +3311,38 @@
       <c r="C59" t="s">
         <v>151</v>
       </c>
-      <c r="D59" t="s">
-        <v>155</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>196</v>
+      <c r="D59">
+        <v>2912</v>
+      </c>
+      <c r="E59" t="s">
+        <v>155</v>
       </c>
       <c r="F59" t="s">
+        <v>196</v>
+      </c>
+      <c r="G59" t="s">
         <v>184</v>
       </c>
-      <c r="G59" t="s">
-        <v>198</v>
-      </c>
-      <c r="H59">
+      <c r="H59" t="s">
+        <v>198</v>
+      </c>
+      <c r="I59">
         <v>9.1</v>
       </c>
-      <c r="I59">
+      <c r="J59">
         <v>100</v>
       </c>
-      <c r="J59" t="s">
-        <v>166</v>
-      </c>
       <c r="K59" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L59" t="s">
+        <v>168</v>
+      </c>
+      <c r="M59" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>20</v>
       </c>
@@ -3179,35 +3352,38 @@
       <c r="C60" t="s">
         <v>44</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60">
+        <v>258</v>
+      </c>
+      <c r="E60" t="s">
         <v>44</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F60" t="s">
+        <v>196</v>
+      </c>
+      <c r="G60" t="s">
         <v>188</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>200</v>
       </c>
-      <c r="H60">
+      <c r="I60">
         <v>6.7</v>
       </c>
-      <c r="I60">
+      <c r="J60">
         <v>3.4</v>
       </c>
-      <c r="J60" t="s">
-        <v>166</v>
-      </c>
       <c r="K60" t="s">
+        <v>166</v>
+      </c>
+      <c r="L60" t="s">
         <v>163</v>
       </c>
-      <c r="L60" t="s">
+      <c r="M60" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>79</v>
       </c>
@@ -3217,35 +3393,38 @@
       <c r="C61" t="s">
         <v>152</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61">
+        <v>68</v>
+      </c>
+      <c r="E61" t="s">
         <v>152</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="F61" t="s">
+        <v>196</v>
+      </c>
+      <c r="G61" t="s">
         <v>194</v>
       </c>
-      <c r="G61" t="s">
-        <v>198</v>
-      </c>
-      <c r="H61">
+      <c r="H61" t="s">
+        <v>198</v>
+      </c>
+      <c r="I61">
         <v>8.1999999999999993</v>
       </c>
-      <c r="I61">
+      <c r="J61">
         <v>82</v>
       </c>
-      <c r="J61" t="s">
-        <v>166</v>
-      </c>
       <c r="K61" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L61" t="s">
+        <v>168</v>
+      </c>
+      <c r="M61" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -3255,35 +3434,38 @@
       <c r="C62" t="s">
         <v>153</v>
       </c>
-      <c r="D62" t="s">
-        <v>155</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>196</v>
+      <c r="D62">
+        <v>151</v>
+      </c>
+      <c r="E62" t="s">
+        <v>155</v>
       </c>
       <c r="F62" t="s">
+        <v>196</v>
+      </c>
+      <c r="G62" t="s">
         <v>185</v>
       </c>
-      <c r="G62" t="s">
-        <v>198</v>
-      </c>
-      <c r="H62">
+      <c r="H62" t="s">
+        <v>198</v>
+      </c>
+      <c r="I62">
         <v>8.1</v>
       </c>
-      <c r="I62">
+      <c r="J62">
         <v>160</v>
       </c>
-      <c r="J62" t="s">
-        <v>166</v>
-      </c>
       <c r="K62" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L62" t="s">
+        <v>168</v>
+      </c>
+      <c r="M62" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -3293,93 +3475,102 @@
       <c r="C63" t="s">
         <v>154</v>
       </c>
-      <c r="D63" t="s">
-        <v>155</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>196</v>
+      <c r="D63">
+        <v>414</v>
+      </c>
+      <c r="E63" t="s">
+        <v>155</v>
       </c>
       <c r="F63" t="s">
+        <v>196</v>
+      </c>
+      <c r="G63" t="s">
         <v>189</v>
       </c>
-      <c r="G63" t="s">
-        <v>198</v>
-      </c>
-      <c r="H63">
+      <c r="H63" t="s">
+        <v>198</v>
+      </c>
+      <c r="I63">
         <v>7.6</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <v>51</v>
       </c>
-      <c r="J63" t="s">
-        <v>166</v>
-      </c>
       <c r="K63" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L63" t="s">
+        <v>168</v>
+      </c>
+      <c r="M63" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C64" t="s">
         <v>181</v>
       </c>
-      <c r="D64" t="s">
-        <v>155</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>196</v>
+      <c r="D64">
+        <v>73</v>
+      </c>
+      <c r="E64" t="s">
+        <v>155</v>
       </c>
       <c r="F64" t="s">
+        <v>196</v>
+      </c>
+      <c r="G64" t="s">
         <v>188</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>199</v>
       </c>
-      <c r="M64" t="s">
+      <c r="N64" t="s">
         <v>181</v>
       </c>
-      <c r="N64" t="s">
+      <c r="O64" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
         <v>176</v>
       </c>
       <c r="C65" t="s">
         <v>176</v>
       </c>
-      <c r="D65" t="s">
-        <v>155</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>196</v>
+      <c r="D65">
+        <v>35</v>
+      </c>
+      <c r="E65" t="s">
+        <v>155</v>
       </c>
       <c r="F65" t="s">
+        <v>196</v>
+      </c>
+      <c r="G65" t="s">
         <v>188</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>199</v>
       </c>
-      <c r="M65" t="s">
+      <c r="N65" t="s">
         <v>176</v>
       </c>
-      <c r="N65" t="s">
+      <c r="O65" t="s">
         <v>174</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N79" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N65">
+  <autoFilter ref="A1:O65" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O65">
     <sortCondition ref="A2:A65"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>